<commit_message>
found some bugs for FrontEndTesting
added the descriptions of the bugs in the FrontEndTesting
</commit_message>
<xml_diff>
--- a/Front End SQA/FrontEndTesting.xlsx
+++ b/Front End SQA/FrontEndTesting.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abel.Abel-PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xavier\Documents\GitHub\UPOD\Front End SQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -115,13 +115,31 @@
   </si>
   <si>
     <t>Frontend - SQA</t>
+  </si>
+  <si>
+    <t>home.html</t>
+  </si>
+  <si>
+    <t>Xavier Kuttamparambil</t>
+  </si>
+  <si>
+    <t>If resize the page and squish it vertically, the search textbox  goes off of the white background box</t>
+  </si>
+  <si>
+    <t>Also, if u squish the page vertically then the search textbox is sometimes on top of the about and create a page buttons so that they can not be clicked</t>
+  </si>
+  <si>
+    <t>If you squish the page horizontally, the about and create a page buttons at the bottom mess up; the create a page button has the word page show up a line below the rest of the buttons even though there is tons of page. Also the buttons are not centered when the page is squished horizontally.</t>
+  </si>
+  <si>
+    <t>The arrow button to search ended up below the search bar on the right side (one of the ways to get the error is to click on the textbox and press enter)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -153,6 +171,13 @@
       <sz val="14"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -238,12 +263,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -272,11 +298,21 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Excel_BuiltIn_Neutral" xfId="2"/>
+  <cellStyles count="4">
+    <cellStyle name="Excel_BuiltIn_Neutral" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,28 +623,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125"/>
-    <col min="2" max="2" width="18.5703125"/>
-    <col min="3" max="3" width="14.140625"/>
-    <col min="4" max="4" width="19.5703125"/>
+    <col min="1" max="1" width="25.5546875"/>
+    <col min="2" max="2" width="18.5546875"/>
+    <col min="3" max="3" width="14.109375"/>
+    <col min="4" max="4" width="19.5546875"/>
     <col min="5" max="5" width="20"/>
-    <col min="6" max="6" width="17.28515625"/>
-    <col min="7" max="7" width="21.28515625"/>
-    <col min="8" max="8" width="20.5703125"/>
-    <col min="9" max="256" width="11.7109375"/>
-    <col min="257" max="1025" width="11.5703125"/>
+    <col min="6" max="6" width="17.33203125"/>
+    <col min="7" max="7" width="21.33203125"/>
+    <col min="8" max="8" width="20.5546875"/>
+    <col min="9" max="256" width="11.6640625"/>
+    <col min="257" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>31</v>
       </c>
@@ -621,7 +657,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
@@ -634,7 +670,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -663,7 +699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -692,7 +728,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -713,7 +749,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -734,7 +770,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -755,7 +791,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -776,7 +812,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -797,7 +833,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
@@ -818,7 +854,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -839,7 +875,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -860,51 +896,91 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="1"/>
+    <row r="13" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4">
+        <v>43089</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4">
+        <v>43089</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:9" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4">
+        <v>43089</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="1"/>
+    <row r="16" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="4">
+        <v>43089</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -915,7 +991,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -926,7 +1002,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -937,7 +1013,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -948,7 +1024,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -959,7 +1035,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -970,7 +1046,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -981,7 +1057,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -992,7 +1068,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1003,7 +1079,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1014,7 +1090,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1025,7 +1101,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1036,7 +1112,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1047,7 +1123,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1058,7 +1134,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1069,7 +1145,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1080,7 +1156,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1091,7 +1167,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1102,7 +1178,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1113,7 +1189,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1124,7 +1200,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1135,7 +1211,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1146,7 +1222,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1157,7 +1233,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1168,7 +1244,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1179,7 +1255,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1190,7 +1266,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1201,7 +1277,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1212,7 +1288,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1223,7 +1299,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1234,7 +1310,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1245,7 +1321,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1256,7 +1332,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1267,7 +1343,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1278,7 +1354,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1289,7 +1365,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1300,7 +1376,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1311,7 +1387,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1322,7 +1398,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1333,7 +1409,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1344,7 +1420,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1355,7 +1431,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1366,7 +1442,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1377,7 +1453,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1388,7 +1464,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1399,7 +1475,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1410,7 +1486,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1421,7 +1497,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1432,7 +1508,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1443,7 +1519,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1454,7 +1530,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1465,7 +1541,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1476,7 +1552,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1487,7 +1563,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1498,7 +1574,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1509,7 +1585,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1520,7 +1596,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1531,7 +1607,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1542,7 +1618,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1553,7 +1629,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1564,7 +1640,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1575,7 +1651,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1586,7 +1662,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1597,7 +1673,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1608,7 +1684,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1619,7 +1695,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1630,7 +1706,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1641,7 +1717,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1652,7 +1728,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1663,7 +1739,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1674,7 +1750,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1685,7 +1761,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1696,7 +1772,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1707,7 +1783,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1723,8 +1799,13 @@
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{74ED26D4-BD79-483E-ACF1-3918FB7A4AA6}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{5EB75C9D-6D15-4981-9E02-4900E1825AFE}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{F2CCDDBF-C25C-4D33-808D-6211FCA3D7DD}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added some more testing to FrontEndTesting
more description on the testing in the file
</commit_message>
<xml_diff>
--- a/Front End SQA/FrontEndTesting.xlsx
+++ b/Front End SQA/FrontEndTesting.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -123,16 +123,25 @@
     <t>Xavier Kuttamparambil</t>
   </si>
   <si>
-    <t>If resize the page and squish it vertically, the search textbox  goes off of the white background box</t>
-  </si>
-  <si>
-    <t>Also, if u squish the page vertically then the search textbox is sometimes on top of the about and create a page buttons so that they can not be clicked</t>
-  </si>
-  <si>
-    <t>If you squish the page horizontally, the about and create a page buttons at the bottom mess up; the create a page button has the word page show up a line below the rest of the buttons even though there is tons of page. Also the buttons are not centered when the page is squished horizontally.</t>
-  </si>
-  <si>
-    <t>The arrow button to search ended up below the search bar on the right side (one of the ways to get the error is to click on the textbox and press enter)</t>
+    <t>The arrow button to search ended up below the search bar on the right side (one of the ways to get the error is to click on the textbox and press enter) (Chrome)</t>
+  </si>
+  <si>
+    <t>If resize the page and squish it vertically, the search textbox  goes off of the white background box (Chrome)</t>
+  </si>
+  <si>
+    <t>Also, if u squish the page vertically then the search textbox is sometimes on top of the about and create a page buttons so that they can not be clicked (Chrome)</t>
+  </si>
+  <si>
+    <t>If you squish the page horizontally, the about and create a page buttons at the bottom mess up; the create a page button has the word page show up a line below the rest of the buttons even though there is tons of page. Also the buttons are not centered when the page is squished horizontally. (Chrome)</t>
+  </si>
+  <si>
+    <t>if you add a section and then click on the textbox which says section title, if you press enter, every added section disappears (Chrome)</t>
+  </si>
+  <si>
+    <t>same as above for the textbox diagram url (Chrome)</t>
+  </si>
+  <si>
+    <t>the add image button also makes every section disappear as well (Chrome)</t>
   </si>
 </sst>
 </file>
@@ -292,12 +301,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -306,6 +309,12 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -626,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,30 +654,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -898,7 +907,7 @@
     </row>
     <row r="13" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>32</v>
@@ -919,7 +928,7 @@
     </row>
     <row r="14" spans="1:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
@@ -940,9 +949,9 @@
     </row>
     <row r="15" spans="1:9" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -959,14 +968,14 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="4">
@@ -980,34 +989,64 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="1"/>
+    <row r="17" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4">
+        <v>43089</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="1"/>
+    <row r="18" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4">
+        <v>43089</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="1"/>
+    <row r="19" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4">
+        <v>43090</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>

</xml_diff>